<commit_message>
2nd project was updated.
</commit_message>
<xml_diff>
--- a/Projects/Project_02_RDB_and_SQL_Data_Analysis_Project_E-Commerce/E-Commerce Data and Customer Retention Analysis with SQL/prod_dimen.xlsx
+++ b/Projects/Project_02_RDB_and_SQL_Data_Analysis_Project_E-Commerce/E-Commerce Data and Customer Retention Analysis with SQL/prod_dimen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CW\MSSQL\DAwSQL\0721\E-Commerce Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sumey\Courses\Bootcamp_Clarusway\Projects\Project_02_RDB_and_SQL_Data_Analysis_Project_E-Commerce\E-Commerce Data and Customer Retention Analysis with SQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3D429133-CB5B-4DA7-83C5-BD4C56EF6E6E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B88DF569-0F2C-4C1F-946C-653A5D2A6B27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="prod_dimen" sheetId="1" r:id="rId1"/>
@@ -145,7 +145,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -645,48 +645,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="%20 - Vurgu1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="%20 - Vurgu2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="%20 - Vurgu3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="%20 - Vurgu4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="%20 - Vurgu5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="%20 - Vurgu6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="%40 - Vurgu1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="%40 - Vurgu2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="%40 - Vurgu3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="%40 - Vurgu4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="%40 - Vurgu5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="%40 - Vurgu6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="%60 - Vurgu1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="%60 - Vurgu2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="%60 - Vurgu3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="%60 - Vurgu4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="%60 - Vurgu5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="%60 - Vurgu6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Açıklama Metni" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Ana Başlık" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Bağlı Hücre" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Başlık 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Başlık 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Başlık 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Başlık 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Çıkış" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Giriş" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Hesaplama" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="İşaretli Hücre" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="İyi" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Kötü" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Not" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Nötr" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Toplam" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Uyarı Metni" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Vurgu1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Vurgu2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Vurgu3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Vurgu4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Vurgu5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Vurgu6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -702,7 +702,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Teması">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -997,17 +997,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1029,7 +1029,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1040,7 +1040,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1051,7 +1051,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1062,7 +1062,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1073,7 +1073,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1095,7 +1095,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1106,7 +1106,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -1117,7 +1117,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1128,7 +1128,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1139,7 +1139,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -1150,7 +1150,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -1161,7 +1161,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -1172,7 +1172,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1183,7 +1183,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>10</v>
       </c>

</xml_diff>